<commit_message>
Identify unit testing scenarios and begin to implement unit testing driver for comprehensive testing of all fields.
</commit_message>
<xml_diff>
--- a/source/tests/test_resources/unit_test_01/input_files/unit_test_01_config.xlsx
+++ b/source/tests/test_resources/unit_test_01/input_files/unit_test_01_config.xlsx
@@ -8,16 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Development/PycharmProjects/ppt-plan-visual/source/tests/test_resources/unit_test_01/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A0517F-2793-FE4B-9102-2390CA155F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFBE74E0-52D2-2C41-A242-6C5D8F3F4498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14140" xr2:uid="{974F07DA-9A00-0C4E-BD47-E61A1ACCDB18}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="4" xr2:uid="{974F07DA-9A00-0C4E-BD47-E61A1ACCDB18}"/>
   </bookViews>
   <sheets>
     <sheet name="PlotConfig" sheetId="1" r:id="rId1"/>
     <sheet name="FormatConfig" sheetId="2" r:id="rId2"/>
     <sheet name="Swimlanes" sheetId="4" r:id="rId3"/>
     <sheet name="Lookup" sheetId="3" r:id="rId4"/>
+    <sheet name="Plan" sheetId="5" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Plan!$D$1:$D$16</definedName>
+    <definedName name="Activity_Shape">PlotConfig!$N$2</definedName>
+    <definedName name="Activity_Text_Width">PlotConfig!$L$2</definedName>
+    <definedName name="Bottom">PlotConfig!$D$2</definedName>
+    <definedName name="Config_Name">PlotConfig!$A$2</definedName>
+    <definedName name="Left">PlotConfig!$C$2</definedName>
+    <definedName name="Max_Date">PlotConfig!$I$2</definedName>
+    <definedName name="Milestone_Shape">PlotConfig!$O$2</definedName>
+    <definedName name="Milestone_Text_Width">PlotConfig!$K$2</definedName>
+    <definedName name="Milestone_Width">PlotConfig!$J$2</definedName>
+    <definedName name="Min_Date">PlotConfig!$H$2</definedName>
+    <definedName name="Right">PlotConfig!$E$2</definedName>
+    <definedName name="Start_Date">Plan!#REF!</definedName>
+    <definedName name="Text_Margin">PlotConfig!$M$2</definedName>
+    <definedName name="Top">PlotConfig!$B$2</definedName>
+    <definedName name="Track_Gap">PlotConfig!$G$2</definedName>
+    <definedName name="Track_Height">PlotConfig!$F$2</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="105">
   <si>
     <t>Top</t>
   </si>
@@ -226,6 +246,132 @@
   </si>
   <si>
     <t>Main</t>
+  </si>
+  <si>
+    <t>Shape</t>
+  </si>
+  <si>
+    <t>Activity 03</t>
+  </si>
+  <si>
+    <t>Activity 02</t>
+  </si>
+  <si>
+    <t>Activity 01</t>
+  </si>
+  <si>
+    <t>Done Format String</t>
+  </si>
+  <si>
+    <t>Format String</t>
+  </si>
+  <si>
+    <t>Text Layout</t>
+  </si>
+  <si>
+    <t>Visual # Tracks To Cover</t>
+  </si>
+  <si>
+    <t>Visual Track # Within Swimlane</t>
+  </si>
+  <si>
+    <t>Visual Swimlane</t>
+  </si>
+  <si>
+    <t>Visual Flag</t>
+  </si>
+  <si>
+    <t>Finish</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Visual Text</t>
+  </si>
+  <si>
+    <t>Task Name</t>
+  </si>
+  <si>
+    <t>Visual Width</t>
+  </si>
+  <si>
+    <t>Num Visual Months</t>
+  </si>
+  <si>
+    <t>Visual Start</t>
+  </si>
+  <si>
+    <t>Visual Finish</t>
+  </si>
+  <si>
+    <t>Day Width</t>
+  </si>
+  <si>
+    <t>Num Visual Days</t>
+  </si>
+  <si>
+    <t>Points Per Cm</t>
+  </si>
+  <si>
+    <t>Activity 04</t>
+  </si>
+  <si>
+    <t>Today</t>
+  </si>
+  <si>
+    <t>Num Shapes</t>
+  </si>
+  <si>
+    <t>Export To Python Test Suite</t>
+  </si>
+  <si>
+    <t>Graphic 1 Top</t>
+  </si>
+  <si>
+    <t>Graphic 1 Days From Left</t>
+  </si>
+  <si>
+    <t>Graphic 1 Left</t>
+  </si>
+  <si>
+    <t>Graphic 1 Export</t>
+  </si>
+  <si>
+    <t>Graphic 2 Days From Left</t>
+  </si>
+  <si>
+    <t>Graphic 2 Top</t>
+  </si>
+  <si>
+    <t>Graphic 2 Left</t>
+  </si>
+  <si>
+    <t>Graphic 2 Export</t>
+  </si>
+  <si>
+    <t>Text Days From Left</t>
+  </si>
+  <si>
+    <t>Text Left</t>
+  </si>
+  <si>
+    <t>Text Export</t>
+  </si>
+  <si>
+    <t>Text Top</t>
+  </si>
+  <si>
+    <t>Graphic 1 Width</t>
+  </si>
+  <si>
+    <t>Graphic 2 Width</t>
+  </si>
+  <si>
+    <t>Text Width</t>
   </si>
 </sst>
 </file>
@@ -285,7 +431,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -293,11 +439,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -312,11 +469,94 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="41">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -391,8 +631,8 @@
     <tableColumn id="4" xr3:uid="{3C82CB69-4E34-DD4B-B0A2-5D794D05BD5F}" name="Right"/>
     <tableColumn id="5" xr3:uid="{33F60B0D-B994-F348-9DAF-DFF7CFD3C78B}" name="Track Height"/>
     <tableColumn id="6" xr3:uid="{AA4C59A1-6ABE-474E-9F4F-9B240F8E7592}" name="Track Gap"/>
-    <tableColumn id="7" xr3:uid="{6E28CFEC-9841-B74D-8D8D-A1FF3D3EAB92}" name="Min Date" dataDxfId="13"/>
-    <tableColumn id="8" xr3:uid="{62CFE236-4C1D-3343-BE40-92CE54A9CD9F}" name="Max Date" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{6E28CFEC-9841-B74D-8D8D-A1FF3D3EAB92}" name="Min Date" dataDxfId="40"/>
+    <tableColumn id="8" xr3:uid="{62CFE236-4C1D-3343-BE40-92CE54A9CD9F}" name="Max Date" dataDxfId="39"/>
     <tableColumn id="9" xr3:uid="{A02F0B81-3578-BB4B-91F7-2CCC8627BEB1}" name="Milestone Width"/>
     <tableColumn id="10" xr3:uid="{FAA856D7-2A25-154B-974D-DE2E1A6BFDA7}" name="Milestone Text Width"/>
     <tableColumn id="11" xr3:uid="{981EC195-CF67-E445-A73F-CEFD0B8E8A7B}" name="Activity Text Width"/>
@@ -405,44 +645,44 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DFA5499-3D72-FD4D-98A8-9A364D6A060E}" name="Table1" displayName="Table1" ref="A1:R9" totalsRowShown="0" headerRowDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DFA5499-3D72-FD4D-98A8-9A364D6A060E}" name="Table1" displayName="Table1" ref="A1:R9" totalsRowShown="0" headerRowDxfId="38">
   <autoFilter ref="A1:R9" xr:uid="{E2FE5099-2205-2446-9D79-AE0D6D124131}"/>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{6F657443-D392-9749-8D22-77937F3594B4}" name="Format Name"/>
     <tableColumn id="18" xr3:uid="{A1AE67FA-1135-E249-8708-8700254B6C5E}" name="Fill Colour Id"/>
-    <tableColumn id="19" xr3:uid="{A4F1695D-EF2E-894B-B345-7232CA996486}" name="Line Colour Id" dataDxfId="10">
+    <tableColumn id="19" xr3:uid="{A4F1695D-EF2E-894B-B345-7232CA996486}" name="Line Colour Id" dataDxfId="37">
       <calculatedColumnFormula>Table1[[#This Row],[Fill Colour Id]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{97389AAA-8E2F-3E46-84CB-DE9C3886C50D}" name="Font Colour Id" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{7A6165F6-6522-4641-AD20-8BFC998689C5}" name="Fill Red" dataDxfId="8">
+    <tableColumn id="20" xr3:uid="{97389AAA-8E2F-3E46-84CB-DE9C3886C50D}" name="Font Colour Id" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{7A6165F6-6522-4641-AD20-8BFC998689C5}" name="Fill Red" dataDxfId="35">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Table1[[#This Row],[Fill Colour Id]],ColourLookup[Id],ColourLookup[Red],"xxx",0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{56111E36-3ADB-5840-8505-3797E3CE7487}" name="Fill Green" dataDxfId="7">
+    <tableColumn id="3" xr3:uid="{56111E36-3ADB-5840-8505-3797E3CE7487}" name="Fill Green" dataDxfId="34">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Table1[[#This Row],[Fill Colour Id]],ColourLookup[Id],ColourLookup[Green],"xxx",0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{D38157EA-874F-2947-9B77-2FE04EF7B6E4}" name="Fill Blue" dataDxfId="6">
+    <tableColumn id="4" xr3:uid="{D38157EA-874F-2947-9B77-2FE04EF7B6E4}" name="Fill Blue" dataDxfId="33">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Table1[[#This Row],[Fill Colour Id]],ColourLookup[Id],ColourLookup[Blue],"xxx",0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{28D5DE83-7F52-6740-8522-D51043E0F7CB}" name="Line Red" dataDxfId="5">
+    <tableColumn id="5" xr3:uid="{28D5DE83-7F52-6740-8522-D51043E0F7CB}" name="Line Red" dataDxfId="32">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Table1[[#This Row],[Line Colour Id]],ColourLookup[Id],ColourLookup[Red],"xxx",0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{24678273-AA26-4148-8430-DDFBC6DB7C13}" name="Line Green" dataDxfId="4">
+    <tableColumn id="6" xr3:uid="{24678273-AA26-4148-8430-DDFBC6DB7C13}" name="Line Green" dataDxfId="31">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Table1[[#This Row],[Line Colour Id]],ColourLookup[Id],ColourLookup[Green],"xxx",0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{5D7C2447-5E29-EC4F-8072-2DC6D9510081}" name="Line Blue" dataDxfId="3">
+    <tableColumn id="7" xr3:uid="{5D7C2447-5E29-EC4F-8072-2DC6D9510081}" name="Line Blue" dataDxfId="30">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Table1[[#This Row],[Line Colour Id]],ColourLookup[Id],ColourLookup[Blue],"xxx",0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{51A1C6F6-14EE-C34E-84CA-DE7646C2274A}" name="Corner Radius (Cm)"/>
     <tableColumn id="9" xr3:uid="{6AB14E61-99B1-B244-BCA2-D862AF5D9E34}" name="Font Size (Pt)"/>
     <tableColumn id="10" xr3:uid="{E2F3AF6B-435F-FC4A-BA6B-5C9307692438}" name="Font Bold"/>
     <tableColumn id="11" xr3:uid="{948FF9F8-AEEA-7440-A660-75BC0C3A997A}" name="Font Italic"/>
-    <tableColumn id="12" xr3:uid="{C4967D4B-CAA6-BC41-B179-E0688B21C6D2}" name="Font Red" dataDxfId="2">
+    <tableColumn id="12" xr3:uid="{C4967D4B-CAA6-BC41-B179-E0688B21C6D2}" name="Font Red" dataDxfId="29">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Table1[[#This Row],[Font Colour Id]],ColourLookup[Id],ColourLookup[Red],"xxx",0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{D242A51C-0847-8443-A306-5735B880BC86}" name="Font Green" dataDxfId="1">
+    <tableColumn id="13" xr3:uid="{D242A51C-0847-8443-A306-5735B880BC86}" name="Font Green" dataDxfId="28">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Table1[[#This Row],[Font Colour Id]],ColourLookup[Id],ColourLookup[Green],"xxx",0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{090E4691-DD9F-C744-92B7-E7EDD88FBC44}" name="Font Blue" dataDxfId="0">
+    <tableColumn id="14" xr3:uid="{090E4691-DD9F-C744-92B7-E7EDD88FBC44}" name="Font Blue" dataDxfId="27">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Table1[[#This Row],[Font Colour Id]],ColourLookup[Id],ColourLookup[Blue],"xxx",0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="17" xr3:uid="{7DA58C0D-D13F-4440-8792-3A5B7AF2004D}" name="Text Vertical Align"/>
@@ -471,6 +711,107 @@
     <tableColumn id="4" xr3:uid="{2C6E550E-4267-5541-BCC7-4E0112706214}" name="Blue"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D389C7E6-D903-204D-A69B-1B9E0C804015}" name="Table16" displayName="Table16" ref="A1:L5" totalsRowShown="0">
+  <autoFilter ref="A1:L5" xr:uid="{94E31D07-C979-BC46-88D8-C174A3004C80}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{CD355BFA-068F-A64A-BFFD-36DB2F65EC92}" name="Task Name"/>
+    <tableColumn id="2" xr3:uid="{2ACCD512-6A3D-FC4C-A65F-1CC1108B4A21}" name="Visual Text"/>
+    <tableColumn id="3" xr3:uid="{01EC07DC-8306-F04F-9046-7DFFA10F5B43}" name="Duration"/>
+    <tableColumn id="4" xr3:uid="{FC6EB61C-7100-B448-9804-603C7E3ABEF3}" name="Start" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{E5228417-109C-A846-AF0B-030C79E6E401}" name="Finish" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{0D84F3B2-D985-3649-8170-9FD8A89B6B7B}" name="Visual Flag"/>
+    <tableColumn id="7" xr3:uid="{4DE64335-5CA3-C14F-836B-CE64DF9836EA}" name="Visual Swimlane"/>
+    <tableColumn id="8" xr3:uid="{CF8C0B08-0C4D-E04F-9D8F-5EE6047AEC86}" name="Visual Track # Within Swimlane"/>
+    <tableColumn id="9" xr3:uid="{0399BB92-883E-C441-B3D6-26B8AAB62A5D}" name="Visual # Tracks To Cover"/>
+    <tableColumn id="10" xr3:uid="{E872D010-2575-154A-B3DC-BC1B261B272B}" name="Text Layout"/>
+    <tableColumn id="11" xr3:uid="{0B2F0106-7954-DA47-9541-E9D49B5C3B31}" name="Format String"/>
+    <tableColumn id="12" xr3:uid="{0339EBEE-CB19-AA47-885D-D16B1966F96D}" name="Done Format String"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{95650287-5270-794F-BE83-228189F68705}" name="Table6" displayName="Table6" ref="O1:AM5" totalsRowShown="0">
+  <autoFilter ref="O1:AM5" xr:uid="{95650287-5270-794F-BE83-228189F68705}"/>
+  <tableColumns count="25">
+    <tableColumn id="1" xr3:uid="{A9D36371-651B-694F-A372-8CF380F533EC}" name="Num Visual Months" dataDxfId="18">
+      <calculatedColumnFormula>1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{52C6E4C9-BF49-3C41-BC4A-3E05A0279392}" name="Num Visual Days" dataDxfId="17">
+      <calculatedColumnFormula>31</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{DC65A63A-00D1-A74D-A035-94831A6C664A}" name="Visual Start" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{DE63D43B-35E2-1D44-8D4E-E5E3760DF168}" name="Visual Finish" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{E8A718C3-23D8-CC4E-B23D-3EBE73F29401}" name="Visual Width" dataDxfId="22">
+      <calculatedColumnFormula>Right-Left</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="12" xr3:uid="{CEF3950D-CB80-6044-B17D-B4B1A8490449}" name="Today" dataDxfId="13">
+      <calculatedColumnFormula>DATE(2021,1,5)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{CB9DFFF7-900F-DF4E-A122-4CFDDA1F4267}" name="Day Width" dataDxfId="15">
+      <calculatedColumnFormula>Table6[[#This Row],[Visual Width]]/Table6[[#This Row],[Num Visual Days]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{4D076DCC-8A79-3943-9AD2-5D30AB20496A}" name="Points Per Cm" dataDxfId="12">
+      <calculatedColumnFormula>360000</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="17" xr3:uid="{87B55787-4D49-F347-ACB4-0F290EE69403}" name="Num Shapes" dataDxfId="16">
+      <calculatedColumnFormula>IF(Table16[[#This Row],[Done Format String]]="",1,2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" xr3:uid="{862BEB4E-A698-DC49-9CAA-B3C33191CD35}" name="Graphic 1 Days From Left" dataDxfId="21">
+      <calculatedColumnFormula>Table16[[#This Row],[Start]]-Table6[[#This Row],[Visual Start]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{63C3F830-DD55-3F47-98B0-94365079404E}" name="Graphic 1 Top" dataDxfId="19">
+      <calculatedColumnFormula>ROUND((Top+(Table16[[#This Row],[Visual Track '# Within Swimlane]]-1)*(Track_Height+Track_Gap))*360000,0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{2B754CAF-25BB-B64C-94DD-01B5925D7AC2}" name="Graphic 1 Left" dataDxfId="20">
+      <calculatedColumnFormula>ROUND((Left+Table6[[#This Row],[Graphic 1 Days From Left]]*Table6[[#This Row],[Day Width]])*Table6[[#This Row],[Points Per Cm]],0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="25" xr3:uid="{3134E155-CCEA-6F4A-9ED4-2DEFCF056A3C}" name="Graphic 1 Width" dataDxfId="0">
+      <calculatedColumnFormula>ROUND(IF(Table6[[#This Row],[Num Shapes]]=1,(Table16[[#This Row],[Finish]]-Table16[[#This Row],[Start]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]],(Table6[[#This Row],[Today]]-Table16[[#This Row],[Start]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]]),0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="22" xr3:uid="{B236D0DC-FC55-3C4D-ABEE-6BEA9A987D2D}" name="Graphic 1 Export" dataDxfId="5">
+      <calculatedColumnFormula>"("&amp;_xlfn.TEXTJOIN(", ",FALSE, Table6[[#This Row],[Graphic 1 Top]:[Graphic 1 Width]])&amp;")"</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="13" xr3:uid="{7FD805D4-814F-2C44-9C12-67258071ABEE}" name="Graphic 2 Days From Left" dataDxfId="14">
+      <calculatedColumnFormula>IF(Table6[[#This Row],[Num Shapes]]=1,"",Table6[[#This Row],[Today]]-Table6[[#This Row],[Visual Start]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="15" xr3:uid="{0ADBBF0F-A9D7-904E-A22E-A87D6B8B8D63}" name="Graphic 2 Top" dataDxfId="11">
+      <calculatedColumnFormula>IF(Table6[[#This Row],[Num Shapes]]=1,"",Table6[[#This Row],[Graphic 1 Top]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="16" xr3:uid="{CFED86F2-256C-E040-9909-052072892A44}" name="Graphic 2 Left" dataDxfId="10">
+      <calculatedColumnFormula>IF(Table6[[#This Row],[Num Shapes]]=1,"",ROUND((Left+Table6[[#This Row],[Graphic 2 Days From Left]]*Table6[[#This Row],[Day Width]])*Table6[[#This Row],[Points Per Cm]],0))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="26" xr3:uid="{11DD9EDA-17D6-C74C-87A5-05BE6C12E5F2}" name="Graphic 2 Width" dataDxfId="1">
+      <calculatedColumnFormula>IF(Table6[[#This Row],[Num Shapes]]=1,"",ROUND((Table16[[#This Row],[Finish]]-Table6[[#This Row],[Today]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]],0))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="23" xr3:uid="{CD08D3CF-34D9-C84F-87E7-D4BBD2711218}" name="Graphic 2 Export" dataDxfId="4">
+      <calculatedColumnFormula>IF(Table6[[#This Row],[Num Shapes]]=1,"","("&amp;_xlfn.TEXTJOIN(", ",FALSE, Table6[[#This Row],[Graphic 2 Top]:[Graphic 2 Width]])&amp;")")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="18" xr3:uid="{DD10CF7E-CB5E-F34B-AB3C-2FEF6D63CFC4}" name="Text Days From Left" dataDxfId="9">
+      <calculatedColumnFormula>Table16[[#This Row],[Start]]-Table6[[#This Row],[Visual Start]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="19" xr3:uid="{251D2619-6DAD-1045-B9A0-8BDEE9B82806}" name="Text Top" dataDxfId="8">
+      <calculatedColumnFormula>ROUND((Top+(Table16[[#This Row],[Visual Track '# Within Swimlane]]-1)*(Track_Height+Track_Gap))*360000,0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="20" xr3:uid="{013082E2-ECB6-D649-A1F4-0CDEE6D50347}" name="Text Left" dataDxfId="7">
+      <calculatedColumnFormula>ROUND((Left+Table6[[#This Row],[Graphic 1 Days From Left]]*Table6[[#This Row],[Day Width]])*Table6[[#This Row],[Points Per Cm]],0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="27" xr3:uid="{CC791E80-A6A4-1C4F-8038-8C67770BD828}" name="Text Width" dataDxfId="2">
+      <calculatedColumnFormula>ROUND((Table16[[#This Row],[Finish]]-Table16[[#This Row],[Start]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]],0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="24" xr3:uid="{BC99535B-484E-854F-AA07-93A4E18F8797}" name="Text Export" dataDxfId="3">
+      <calculatedColumnFormula>"("&amp;_xlfn.TEXTJOIN(", ",FALSE, Table6[[#This Row],[Text Top]:[Text Width]])&amp;")"</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="21" xr3:uid="{62743F9D-847D-3F4E-BC1E-B073C3B3E68A}" name="Export To Python Test Suite" dataDxfId="6">
+      <calculatedColumnFormula>"("&amp;"""Activity"""&amp;", "&amp;""""&amp;Table16[[#This Row],[Task Name]]&amp;""""&amp;", "&amp;"["&amp;_xlfn.TEXTJOIN(", ",TRUE, Table6[[#This Row],[Graphic 1 Export]],Table6[[#This Row],[Graphic 2 Export]],Table6[[#This Row],[Text Export]])&amp;"]"&amp;"),"</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -774,8 +1115,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -842,10 +1183,10 @@
         <v>41</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D2">
         <v>19</v>
@@ -1754,6 +2095,682 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F13C002-A285-3448-A960-87C1D30D67A8}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:AM5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="182" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.5" customWidth="1"/>
+    <col min="14" max="14" width="3.33203125" customWidth="1"/>
+    <col min="15" max="15" width="20" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="25" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.1640625" customWidth="1"/>
+    <col min="28" max="28" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="25" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.1640625" customWidth="1"/>
+    <col min="33" max="33" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11" customWidth="1"/>
+    <col min="38" max="38" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="97.83203125" bestFit="1" customWidth="1"/>
+    <col min="40" max="106" width="3.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O1" t="s">
+        <v>80</v>
+      </c>
+      <c r="P1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>81</v>
+      </c>
+      <c r="R1" t="s">
+        <v>82</v>
+      </c>
+      <c r="S1" t="s">
+        <v>79</v>
+      </c>
+      <c r="T1" t="s">
+        <v>87</v>
+      </c>
+      <c r="U1" t="s">
+        <v>83</v>
+      </c>
+      <c r="V1" t="s">
+        <v>85</v>
+      </c>
+      <c r="W1" t="s">
+        <v>88</v>
+      </c>
+      <c r="X1" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="5">
+        <v>44197</v>
+      </c>
+      <c r="E2" s="5">
+        <v>44226</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="O2">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <f>31</f>
+        <v>31</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>44197</v>
+      </c>
+      <c r="R2" s="5">
+        <v>44227</v>
+      </c>
+      <c r="S2" s="7">
+        <f>Right-Left</f>
+        <v>31.869999999999997</v>
+      </c>
+      <c r="T2" s="5">
+        <f t="shared" ref="T2:T5" si="0">DATE(2021,1,5)</f>
+        <v>44201</v>
+      </c>
+      <c r="U2" s="7">
+        <f>Table6[[#This Row],[Visual Width]]/Table6[[#This Row],[Num Visual Days]]</f>
+        <v>1.0280645161290323</v>
+      </c>
+      <c r="V2" s="7">
+        <f t="shared" ref="V2:V4" si="1">360000</f>
+        <v>360000</v>
+      </c>
+      <c r="W2" s="7">
+        <f>IF(Table16[[#This Row],[Done Format String]]="",1,2)</f>
+        <v>1</v>
+      </c>
+      <c r="X2" s="7">
+        <f>Table16[[#This Row],[Start]]-Table6[[#This Row],[Visual Start]]</f>
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <f>ROUND((Top+(Table16[[#This Row],[Visual Track '# Within Swimlane]]-1)*(Track_Height+Track_Gap))*360000,0)</f>
+        <v>360000</v>
+      </c>
+      <c r="Z2">
+        <f>ROUND((Left+Table6[[#This Row],[Graphic 1 Days From Left]]*Table6[[#This Row],[Day Width]])*Table6[[#This Row],[Points Per Cm]],0)</f>
+        <v>720000</v>
+      </c>
+      <c r="AA2">
+        <f>ROUND(IF(Table6[[#This Row],[Num Shapes]]=1,(Table16[[#This Row],[Finish]]-Table16[[#This Row],[Start]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]],(Table6[[#This Row],[Today]]-Table16[[#This Row],[Start]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]]),0)</f>
+        <v>11103097</v>
+      </c>
+      <c r="AB2" t="str">
+        <f>"("&amp;_xlfn.TEXTJOIN(", ",FALSE, Table6[[#This Row],[Graphic 1 Top]:[Graphic 1 Width]])&amp;")"</f>
+        <v>(360000, 720000, 11103097)</v>
+      </c>
+      <c r="AC2" s="7" t="str">
+        <f>IF(Table6[[#This Row],[Num Shapes]]=1,"",Table6[[#This Row],[Today]]-Table6[[#This Row],[Visual Start]])</f>
+        <v/>
+      </c>
+      <c r="AD2" s="7" t="str">
+        <f>IF(Table6[[#This Row],[Num Shapes]]=1,"",Table6[[#This Row],[Graphic 1 Top]])</f>
+        <v/>
+      </c>
+      <c r="AE2" s="7" t="str">
+        <f>IF(Table6[[#This Row],[Num Shapes]]=1,"",ROUND((Left+Table6[[#This Row],[Graphic 2 Days From Left]]*Table6[[#This Row],[Day Width]])*Table6[[#This Row],[Points Per Cm]],0))</f>
+        <v/>
+      </c>
+      <c r="AF2" s="7" t="str">
+        <f>IF(Table6[[#This Row],[Num Shapes]]=1,"",ROUND((Table16[[#This Row],[Finish]]-Table6[[#This Row],[Today]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]],0))</f>
+        <v/>
+      </c>
+      <c r="AG2" t="str">
+        <f>IF(Table6[[#This Row],[Num Shapes]]=1,"","("&amp;_xlfn.TEXTJOIN(", ",FALSE, Table6[[#This Row],[Graphic 2 Top]:[Graphic 2 Width]])&amp;")")</f>
+        <v/>
+      </c>
+      <c r="AH2" s="7">
+        <f>Table16[[#This Row],[Start]]-Table6[[#This Row],[Visual Start]]</f>
+        <v>0</v>
+      </c>
+      <c r="AI2" s="7">
+        <f>ROUND((Top+(Table16[[#This Row],[Visual Track '# Within Swimlane]]-1)*(Track_Height+Track_Gap))*360000,0)</f>
+        <v>360000</v>
+      </c>
+      <c r="AJ2" s="7">
+        <f>ROUND((Left+Table6[[#This Row],[Graphic 1 Days From Left]]*Table6[[#This Row],[Day Width]])*Table6[[#This Row],[Points Per Cm]],0)</f>
+        <v>720000</v>
+      </c>
+      <c r="AK2" s="7">
+        <f>ROUND((Table16[[#This Row],[Finish]]-Table16[[#This Row],[Start]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]],0)</f>
+        <v>11103097</v>
+      </c>
+      <c r="AL2" s="7" t="str">
+        <f>"("&amp;_xlfn.TEXTJOIN(", ",FALSE, Table6[[#This Row],[Text Top]:[Text Width]])&amp;")"</f>
+        <v>(360000, 720000, 11103097)</v>
+      </c>
+      <c r="AM2" s="7" t="str">
+        <f>"("&amp;"""Activity"""&amp;", "&amp;""""&amp;Table16[[#This Row],[Task Name]]&amp;""""&amp;", "&amp;"["&amp;_xlfn.TEXTJOIN(", ",TRUE, Table6[[#This Row],[Graphic 1 Export]],Table6[[#This Row],[Graphic 2 Export]],Table6[[#This Row],[Text Export]])&amp;"]"&amp;"),"</f>
+        <v>("Activity", "Activity 01", [(360000, 720000, 11103097), (360000, 720000, 11103097)]),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="5">
+        <v>44197</v>
+      </c>
+      <c r="E3" s="5">
+        <v>44226</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="J3" t="s">
+        <v>63</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="O3">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <f>31</f>
+        <v>31</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>44197</v>
+      </c>
+      <c r="R3" s="5">
+        <v>44227</v>
+      </c>
+      <c r="S3" s="7">
+        <f>Right-Left</f>
+        <v>31.869999999999997</v>
+      </c>
+      <c r="T3" s="5">
+        <f t="shared" si="0"/>
+        <v>44201</v>
+      </c>
+      <c r="U3" s="7">
+        <f>Table6[[#This Row],[Visual Width]]/Table6[[#This Row],[Num Visual Days]]</f>
+        <v>1.0280645161290323</v>
+      </c>
+      <c r="V3" s="7">
+        <f t="shared" si="1"/>
+        <v>360000</v>
+      </c>
+      <c r="W3" s="7">
+        <f>IF(Table16[[#This Row],[Done Format String]]="",1,2)</f>
+        <v>1</v>
+      </c>
+      <c r="X3" s="7">
+        <f>Table16[[#This Row],[Start]]-Table6[[#This Row],[Visual Start]]</f>
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <f>ROUND((Top+(Table16[[#This Row],[Visual Track '# Within Swimlane]]-1)*(Track_Height+Track_Gap))*360000,0)</f>
+        <v>576000</v>
+      </c>
+      <c r="Z3">
+        <f>ROUND((Left+Table6[[#This Row],[Graphic 1 Days From Left]]*Table6[[#This Row],[Day Width]])*Table6[[#This Row],[Points Per Cm]],0)</f>
+        <v>720000</v>
+      </c>
+      <c r="AA3">
+        <f>ROUND(IF(Table6[[#This Row],[Num Shapes]]=1,(Table16[[#This Row],[Finish]]-Table16[[#This Row],[Start]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]],(Table6[[#This Row],[Today]]-Table16[[#This Row],[Start]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]]),0)</f>
+        <v>11103097</v>
+      </c>
+      <c r="AB3" t="str">
+        <f>"("&amp;_xlfn.TEXTJOIN(", ",FALSE, Table6[[#This Row],[Graphic 1 Top]:[Graphic 1 Width]])&amp;")"</f>
+        <v>(576000, 720000, 11103097)</v>
+      </c>
+      <c r="AC3" s="7" t="str">
+        <f>IF(Table6[[#This Row],[Num Shapes]]=1,"",Table6[[#This Row],[Today]]-Table6[[#This Row],[Visual Start]])</f>
+        <v/>
+      </c>
+      <c r="AD3" s="7" t="str">
+        <f>IF(Table6[[#This Row],[Num Shapes]]=1,"",Table6[[#This Row],[Graphic 1 Top]])</f>
+        <v/>
+      </c>
+      <c r="AE3" s="7" t="str">
+        <f>IF(Table6[[#This Row],[Num Shapes]]=1,"",ROUND((Left+Table6[[#This Row],[Graphic 2 Days From Left]]*Table6[[#This Row],[Day Width]])*Table6[[#This Row],[Points Per Cm]],0))</f>
+        <v/>
+      </c>
+      <c r="AF3" s="7" t="str">
+        <f>IF(Table6[[#This Row],[Num Shapes]]=1,"",ROUND((Table16[[#This Row],[Finish]]-Table6[[#This Row],[Today]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]],0))</f>
+        <v/>
+      </c>
+      <c r="AG3" s="7" t="str">
+        <f>IF(Table6[[#This Row],[Num Shapes]]=1,"","("&amp;_xlfn.TEXTJOIN(", ",FALSE, Table6[[#This Row],[Graphic 2 Top]:[Graphic 2 Width]])&amp;")")</f>
+        <v/>
+      </c>
+      <c r="AH3" s="7">
+        <f>Table16[[#This Row],[Start]]-Table6[[#This Row],[Visual Start]]</f>
+        <v>0</v>
+      </c>
+      <c r="AI3" s="7">
+        <f>ROUND((Top+(Table16[[#This Row],[Visual Track '# Within Swimlane]]-1)*(Track_Height+Track_Gap))*360000,0)</f>
+        <v>576000</v>
+      </c>
+      <c r="AJ3" s="7">
+        <f>ROUND((Left+Table6[[#This Row],[Graphic 1 Days From Left]]*Table6[[#This Row],[Day Width]])*Table6[[#This Row],[Points Per Cm]],0)</f>
+        <v>720000</v>
+      </c>
+      <c r="AK3" s="7">
+        <f>ROUND((Table16[[#This Row],[Finish]]-Table16[[#This Row],[Start]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]],0)</f>
+        <v>11103097</v>
+      </c>
+      <c r="AL3" s="7" t="str">
+        <f>"("&amp;_xlfn.TEXTJOIN(", ",FALSE, Table6[[#This Row],[Text Top]:[Text Width]])&amp;")"</f>
+        <v>(576000, 720000, 11103097)</v>
+      </c>
+      <c r="AM3" s="7" t="str">
+        <f>"("&amp;"""Activity"""&amp;", "&amp;""""&amp;Table16[[#This Row],[Task Name]]&amp;""""&amp;", "&amp;"["&amp;_xlfn.TEXTJOIN(", ",TRUE, Table6[[#This Row],[Graphic 1 Export]],Table6[[#This Row],[Graphic 2 Export]],Table6[[#This Row],[Text Export]])&amp;"]"&amp;"),"</f>
+        <v>("Activity", "Activity 02", [(576000, 720000, 11103097), (576000, 720000, 11103097)]),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="5">
+        <v>44198</v>
+      </c>
+      <c r="E4" s="5">
+        <v>44226</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="J4" t="s">
+        <v>63</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="O4">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <f>31</f>
+        <v>31</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>44197</v>
+      </c>
+      <c r="R4" s="5">
+        <v>44227</v>
+      </c>
+      <c r="S4" s="7">
+        <f>Right-Left</f>
+        <v>31.869999999999997</v>
+      </c>
+      <c r="T4" s="5">
+        <f t="shared" si="0"/>
+        <v>44201</v>
+      </c>
+      <c r="U4" s="7">
+        <f>Table6[[#This Row],[Visual Width]]/Table6[[#This Row],[Num Visual Days]]</f>
+        <v>1.0280645161290323</v>
+      </c>
+      <c r="V4" s="7">
+        <f t="shared" si="1"/>
+        <v>360000</v>
+      </c>
+      <c r="W4" s="7">
+        <f>IF(Table16[[#This Row],[Done Format String]]="",1,2)</f>
+        <v>1</v>
+      </c>
+      <c r="X4" s="7">
+        <f>Table16[[#This Row],[Start]]-Table6[[#This Row],[Visual Start]]</f>
+        <v>1</v>
+      </c>
+      <c r="Y4">
+        <f>ROUND((Top+(Table16[[#This Row],[Visual Track '# Within Swimlane]]-1)*(Track_Height+Track_Gap))*360000,0)</f>
+        <v>792000</v>
+      </c>
+      <c r="Z4">
+        <f>ROUND((Left+Table6[[#This Row],[Graphic 1 Days From Left]]*Table6[[#This Row],[Day Width]])*Table6[[#This Row],[Points Per Cm]],0)</f>
+        <v>1090103</v>
+      </c>
+      <c r="AA4">
+        <f>ROUND(IF(Table6[[#This Row],[Num Shapes]]=1,(Table16[[#This Row],[Finish]]-Table16[[#This Row],[Start]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]],(Table6[[#This Row],[Today]]-Table16[[#This Row],[Start]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]]),0)</f>
+        <v>10732994</v>
+      </c>
+      <c r="AB4" t="str">
+        <f>"("&amp;_xlfn.TEXTJOIN(", ",FALSE, Table6[[#This Row],[Graphic 1 Top]:[Graphic 1 Width]])&amp;")"</f>
+        <v>(792000, 1090103, 10732994)</v>
+      </c>
+      <c r="AC4" s="7" t="str">
+        <f>IF(Table6[[#This Row],[Num Shapes]]=1,"",Table6[[#This Row],[Today]]-Table6[[#This Row],[Visual Start]])</f>
+        <v/>
+      </c>
+      <c r="AD4" s="7" t="str">
+        <f>IF(Table6[[#This Row],[Num Shapes]]=1,"",Table6[[#This Row],[Graphic 1 Top]])</f>
+        <v/>
+      </c>
+      <c r="AE4" s="7" t="str">
+        <f>IF(Table6[[#This Row],[Num Shapes]]=1,"",ROUND((Left+Table6[[#This Row],[Graphic 2 Days From Left]]*Table6[[#This Row],[Day Width]])*Table6[[#This Row],[Points Per Cm]],0))</f>
+        <v/>
+      </c>
+      <c r="AF4" s="7" t="str">
+        <f>IF(Table6[[#This Row],[Num Shapes]]=1,"",ROUND((Table16[[#This Row],[Finish]]-Table6[[#This Row],[Today]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]],0))</f>
+        <v/>
+      </c>
+      <c r="AG4" s="7" t="str">
+        <f>IF(Table6[[#This Row],[Num Shapes]]=1,"","("&amp;_xlfn.TEXTJOIN(", ",FALSE, Table6[[#This Row],[Graphic 2 Top]:[Graphic 2 Width]])&amp;")")</f>
+        <v/>
+      </c>
+      <c r="AH4" s="7">
+        <f>Table16[[#This Row],[Start]]-Table6[[#This Row],[Visual Start]]</f>
+        <v>1</v>
+      </c>
+      <c r="AI4" s="7">
+        <f>ROUND((Top+(Table16[[#This Row],[Visual Track '# Within Swimlane]]-1)*(Track_Height+Track_Gap))*360000,0)</f>
+        <v>792000</v>
+      </c>
+      <c r="AJ4" s="7">
+        <f>ROUND((Left+Table6[[#This Row],[Graphic 1 Days From Left]]*Table6[[#This Row],[Day Width]])*Table6[[#This Row],[Points Per Cm]],0)</f>
+        <v>1090103</v>
+      </c>
+      <c r="AK4" s="7">
+        <f>ROUND((Table16[[#This Row],[Finish]]-Table16[[#This Row],[Start]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]],0)</f>
+        <v>10732994</v>
+      </c>
+      <c r="AL4" s="7" t="str">
+        <f>"("&amp;_xlfn.TEXTJOIN(", ",FALSE, Table6[[#This Row],[Text Top]:[Text Width]])&amp;")"</f>
+        <v>(792000, 1090103, 10732994)</v>
+      </c>
+      <c r="AM4" s="7" t="str">
+        <f>"("&amp;"""Activity"""&amp;", "&amp;""""&amp;Table16[[#This Row],[Task Name]]&amp;""""&amp;", "&amp;"["&amp;_xlfn.TEXTJOIN(", ",TRUE, Table6[[#This Row],[Graphic 1 Export]],Table6[[#This Row],[Graphic 2 Export]],Table6[[#This Row],[Text Export]])&amp;"]"&amp;"),"</f>
+        <v>("Activity", "Activity 03", [(792000, 1090103, 10732994), (792000, 1090103, 10732994)]),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="5">
+        <v>44199</v>
+      </c>
+      <c r="E5" s="5">
+        <v>44216</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="J5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="O5">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="P5" s="7">
+        <f>31</f>
+        <v>31</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>44197</v>
+      </c>
+      <c r="R5" s="5">
+        <v>44227</v>
+      </c>
+      <c r="S5" s="7">
+        <f>Right-Left</f>
+        <v>31.869999999999997</v>
+      </c>
+      <c r="T5" s="5">
+        <f t="shared" si="0"/>
+        <v>44201</v>
+      </c>
+      <c r="U5" s="7">
+        <f>Table6[[#This Row],[Visual Width]]/Table6[[#This Row],[Num Visual Days]]</f>
+        <v>1.0280645161290323</v>
+      </c>
+      <c r="V5" s="7">
+        <f>360000</f>
+        <v>360000</v>
+      </c>
+      <c r="W5" s="7">
+        <f>IF(Table16[[#This Row],[Done Format String]]="",1,2)</f>
+        <v>2</v>
+      </c>
+      <c r="X5" s="7">
+        <f>Table16[[#This Row],[Start]]-Table6[[#This Row],[Visual Start]]</f>
+        <v>2</v>
+      </c>
+      <c r="Y5" s="7">
+        <f>ROUND((Top+(Table16[[#This Row],[Visual Track '# Within Swimlane]]-1)*(Track_Height+Track_Gap))*360000,0)</f>
+        <v>1008000</v>
+      </c>
+      <c r="Z5" s="7">
+        <f>ROUND((Left+Table6[[#This Row],[Graphic 1 Days From Left]]*Table6[[#This Row],[Day Width]])*Table6[[#This Row],[Points Per Cm]],0)</f>
+        <v>1460206</v>
+      </c>
+      <c r="AA5" s="7">
+        <f>ROUND(IF(Table6[[#This Row],[Num Shapes]]=1,(Table16[[#This Row],[Finish]]-Table16[[#This Row],[Start]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]],(Table6[[#This Row],[Today]]-Table16[[#This Row],[Start]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]]),0)</f>
+        <v>1110310</v>
+      </c>
+      <c r="AB5" s="7" t="str">
+        <f>"("&amp;_xlfn.TEXTJOIN(", ",FALSE, Table6[[#This Row],[Graphic 1 Top]:[Graphic 1 Width]])&amp;")"</f>
+        <v>(1008000, 1460206, 1110310)</v>
+      </c>
+      <c r="AC5" s="7">
+        <f>IF(Table6[[#This Row],[Num Shapes]]=1,"",Table6[[#This Row],[Today]]-Table6[[#This Row],[Visual Start]])</f>
+        <v>4</v>
+      </c>
+      <c r="AD5" s="7">
+        <f>IF(Table6[[#This Row],[Num Shapes]]=1,"",Table6[[#This Row],[Graphic 1 Top]])</f>
+        <v>1008000</v>
+      </c>
+      <c r="AE5" s="7">
+        <f>IF(Table6[[#This Row],[Num Shapes]]=1,"",ROUND((Left+Table6[[#This Row],[Graphic 2 Days From Left]]*Table6[[#This Row],[Day Width]])*Table6[[#This Row],[Points Per Cm]],0))</f>
+        <v>2200413</v>
+      </c>
+      <c r="AF5" s="7">
+        <f>IF(Table6[[#This Row],[Num Shapes]]=1,"",ROUND((Table16[[#This Row],[Finish]]-Table6[[#This Row],[Today]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]],0))</f>
+        <v>5921652</v>
+      </c>
+      <c r="AG5" s="7" t="str">
+        <f>IF(Table6[[#This Row],[Num Shapes]]=1,"","("&amp;_xlfn.TEXTJOIN(", ",FALSE, Table6[[#This Row],[Graphic 2 Top]:[Graphic 2 Width]])&amp;")")</f>
+        <v>(1008000, 2200413, 5921652)</v>
+      </c>
+      <c r="AH5" s="7">
+        <f>Table16[[#This Row],[Start]]-Table6[[#This Row],[Visual Start]]</f>
+        <v>2</v>
+      </c>
+      <c r="AI5" s="7">
+        <f>ROUND((Top+(Table16[[#This Row],[Visual Track '# Within Swimlane]]-1)*(Track_Height+Track_Gap))*360000,0)</f>
+        <v>1008000</v>
+      </c>
+      <c r="AJ5" s="7">
+        <f>ROUND((Left+Table6[[#This Row],[Graphic 1 Days From Left]]*Table6[[#This Row],[Day Width]])*Table6[[#This Row],[Points Per Cm]],0)</f>
+        <v>1460206</v>
+      </c>
+      <c r="AK5" s="7">
+        <f>ROUND((Table16[[#This Row],[Finish]]-Table16[[#This Row],[Start]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]],0)</f>
+        <v>6661858</v>
+      </c>
+      <c r="AL5" s="7" t="str">
+        <f>"("&amp;_xlfn.TEXTJOIN(", ",FALSE, Table6[[#This Row],[Text Top]:[Text Width]])&amp;")"</f>
+        <v>(1008000, 1460206, 6661858)</v>
+      </c>
+      <c r="AM5" s="7" t="str">
+        <f>"("&amp;"""Activity"""&amp;", "&amp;""""&amp;Table16[[#This Row],[Task Name]]&amp;""""&amp;", "&amp;"["&amp;_xlfn.TEXTJOIN(", ",TRUE, Table6[[#This Row],[Graphic 1 Export]],Table6[[#This Row],[Graphic 2 Export]],Table6[[#This Row],[Text Export]])&amp;"]"&amp;"),"</f>
+        <v>("Activity", "Activity 04", [(1008000, 1460206, 1110310), (1008000, 2200413, 5921652), (1008000, 1460206, 6661858)]),</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="28" fitToHeight="0" orientation="landscape" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Added height to unit tests
Fixed bug in test calculation of width for graphic 1 when there are two graphics.
</commit_message>
<xml_diff>
--- a/source/tests/test_resources/unit_test_01/input_files/unit_test_01_config.xlsx
+++ b/source/tests/test_resources/unit_test_01/input_files/unit_test_01_config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Development/PycharmProjects/ppt-plan-visual/source/tests/test_resources/unit_test_01/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFBE74E0-52D2-2C41-A242-6C5D8F3F4498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E99ECA-6C87-2646-8A8C-C9B6CA4528BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="4" xr2:uid="{974F07DA-9A00-0C4E-BD47-E61A1ACCDB18}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="108">
   <si>
     <t>Top</t>
   </si>
@@ -326,9 +326,6 @@
     <t>Num Shapes</t>
   </si>
   <si>
-    <t>Export To Python Test Suite</t>
-  </si>
-  <si>
     <t>Graphic 1 Top</t>
   </si>
   <si>
@@ -372,6 +369,18 @@
   </si>
   <si>
     <t>Text Width</t>
+  </si>
+  <si>
+    <t>Graphic 1 Top, Graphic 1 Left, Graphic 1 Width, Graphic 2 Top, Graphic 2 Left, Graphic 2 Width, Text Top, Text Left, Text Width</t>
+  </si>
+  <si>
+    <t>Graphic 1 Height</t>
+  </si>
+  <si>
+    <t>Text Height</t>
+  </si>
+  <si>
+    <t>Graphic 2 Height</t>
   </si>
 </sst>
 </file>
@@ -475,7 +484,13 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="41">
+  <dxfs count="43">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -631,8 +646,8 @@
     <tableColumn id="4" xr3:uid="{3C82CB69-4E34-DD4B-B0A2-5D794D05BD5F}" name="Right"/>
     <tableColumn id="5" xr3:uid="{33F60B0D-B994-F348-9DAF-DFF7CFD3C78B}" name="Track Height"/>
     <tableColumn id="6" xr3:uid="{AA4C59A1-6ABE-474E-9F4F-9B240F8E7592}" name="Track Gap"/>
-    <tableColumn id="7" xr3:uid="{6E28CFEC-9841-B74D-8D8D-A1FF3D3EAB92}" name="Min Date" dataDxfId="40"/>
-    <tableColumn id="8" xr3:uid="{62CFE236-4C1D-3343-BE40-92CE54A9CD9F}" name="Max Date" dataDxfId="39"/>
+    <tableColumn id="7" xr3:uid="{6E28CFEC-9841-B74D-8D8D-A1FF3D3EAB92}" name="Min Date" dataDxfId="42"/>
+    <tableColumn id="8" xr3:uid="{62CFE236-4C1D-3343-BE40-92CE54A9CD9F}" name="Max Date" dataDxfId="41"/>
     <tableColumn id="9" xr3:uid="{A02F0B81-3578-BB4B-91F7-2CCC8627BEB1}" name="Milestone Width"/>
     <tableColumn id="10" xr3:uid="{FAA856D7-2A25-154B-974D-DE2E1A6BFDA7}" name="Milestone Text Width"/>
     <tableColumn id="11" xr3:uid="{981EC195-CF67-E445-A73F-CEFD0B8E8A7B}" name="Activity Text Width"/>
@@ -645,44 +660,44 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DFA5499-3D72-FD4D-98A8-9A364D6A060E}" name="Table1" displayName="Table1" ref="A1:R9" totalsRowShown="0" headerRowDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DFA5499-3D72-FD4D-98A8-9A364D6A060E}" name="Table1" displayName="Table1" ref="A1:R9" totalsRowShown="0" headerRowDxfId="40">
   <autoFilter ref="A1:R9" xr:uid="{E2FE5099-2205-2446-9D79-AE0D6D124131}"/>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{6F657443-D392-9749-8D22-77937F3594B4}" name="Format Name"/>
     <tableColumn id="18" xr3:uid="{A1AE67FA-1135-E249-8708-8700254B6C5E}" name="Fill Colour Id"/>
-    <tableColumn id="19" xr3:uid="{A4F1695D-EF2E-894B-B345-7232CA996486}" name="Line Colour Id" dataDxfId="37">
+    <tableColumn id="19" xr3:uid="{A4F1695D-EF2E-894B-B345-7232CA996486}" name="Line Colour Id" dataDxfId="39">
       <calculatedColumnFormula>Table1[[#This Row],[Fill Colour Id]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{97389AAA-8E2F-3E46-84CB-DE9C3886C50D}" name="Font Colour Id" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{7A6165F6-6522-4641-AD20-8BFC998689C5}" name="Fill Red" dataDxfId="35">
+    <tableColumn id="20" xr3:uid="{97389AAA-8E2F-3E46-84CB-DE9C3886C50D}" name="Font Colour Id" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{7A6165F6-6522-4641-AD20-8BFC998689C5}" name="Fill Red" dataDxfId="37">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Table1[[#This Row],[Fill Colour Id]],ColourLookup[Id],ColourLookup[Red],"xxx",0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{56111E36-3ADB-5840-8505-3797E3CE7487}" name="Fill Green" dataDxfId="34">
+    <tableColumn id="3" xr3:uid="{56111E36-3ADB-5840-8505-3797E3CE7487}" name="Fill Green" dataDxfId="36">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Table1[[#This Row],[Fill Colour Id]],ColourLookup[Id],ColourLookup[Green],"xxx",0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{D38157EA-874F-2947-9B77-2FE04EF7B6E4}" name="Fill Blue" dataDxfId="33">
+    <tableColumn id="4" xr3:uid="{D38157EA-874F-2947-9B77-2FE04EF7B6E4}" name="Fill Blue" dataDxfId="35">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Table1[[#This Row],[Fill Colour Id]],ColourLookup[Id],ColourLookup[Blue],"xxx",0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{28D5DE83-7F52-6740-8522-D51043E0F7CB}" name="Line Red" dataDxfId="32">
+    <tableColumn id="5" xr3:uid="{28D5DE83-7F52-6740-8522-D51043E0F7CB}" name="Line Red" dataDxfId="34">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Table1[[#This Row],[Line Colour Id]],ColourLookup[Id],ColourLookup[Red],"xxx",0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{24678273-AA26-4148-8430-DDFBC6DB7C13}" name="Line Green" dataDxfId="31">
+    <tableColumn id="6" xr3:uid="{24678273-AA26-4148-8430-DDFBC6DB7C13}" name="Line Green" dataDxfId="33">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Table1[[#This Row],[Line Colour Id]],ColourLookup[Id],ColourLookup[Green],"xxx",0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{5D7C2447-5E29-EC4F-8072-2DC6D9510081}" name="Line Blue" dataDxfId="30">
+    <tableColumn id="7" xr3:uid="{5D7C2447-5E29-EC4F-8072-2DC6D9510081}" name="Line Blue" dataDxfId="32">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Table1[[#This Row],[Line Colour Id]],ColourLookup[Id],ColourLookup[Blue],"xxx",0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{51A1C6F6-14EE-C34E-84CA-DE7646C2274A}" name="Corner Radius (Cm)"/>
     <tableColumn id="9" xr3:uid="{6AB14E61-99B1-B244-BCA2-D862AF5D9E34}" name="Font Size (Pt)"/>
     <tableColumn id="10" xr3:uid="{E2F3AF6B-435F-FC4A-BA6B-5C9307692438}" name="Font Bold"/>
     <tableColumn id="11" xr3:uid="{948FF9F8-AEEA-7440-A660-75BC0C3A997A}" name="Font Italic"/>
-    <tableColumn id="12" xr3:uid="{C4967D4B-CAA6-BC41-B179-E0688B21C6D2}" name="Font Red" dataDxfId="29">
+    <tableColumn id="12" xr3:uid="{C4967D4B-CAA6-BC41-B179-E0688B21C6D2}" name="Font Red" dataDxfId="31">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Table1[[#This Row],[Font Colour Id]],ColourLookup[Id],ColourLookup[Red],"xxx",0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{D242A51C-0847-8443-A306-5735B880BC86}" name="Font Green" dataDxfId="28">
+    <tableColumn id="13" xr3:uid="{D242A51C-0847-8443-A306-5735B880BC86}" name="Font Green" dataDxfId="30">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Table1[[#This Row],[Font Colour Id]],ColourLookup[Id],ColourLookup[Green],"xxx",0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{090E4691-DD9F-C744-92B7-E7EDD88FBC44}" name="Font Blue" dataDxfId="27">
+    <tableColumn id="14" xr3:uid="{090E4691-DD9F-C744-92B7-E7EDD88FBC44}" name="Font Blue" dataDxfId="29">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Table1[[#This Row],[Font Colour Id]],ColourLookup[Id],ColourLookup[Blue],"xxx",0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="17" xr3:uid="{7DA58C0D-D13F-4440-8792-3A5B7AF2004D}" name="Text Vertical Align"/>
@@ -721,8 +736,8 @@
     <tableColumn id="1" xr3:uid="{CD355BFA-068F-A64A-BFFD-36DB2F65EC92}" name="Task Name"/>
     <tableColumn id="2" xr3:uid="{2ACCD512-6A3D-FC4C-A65F-1CC1108B4A21}" name="Visual Text"/>
     <tableColumn id="3" xr3:uid="{01EC07DC-8306-F04F-9046-7DFFA10F5B43}" name="Duration"/>
-    <tableColumn id="4" xr3:uid="{FC6EB61C-7100-B448-9804-603C7E3ABEF3}" name="Start" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{E5228417-109C-A846-AF0B-030C79E6E401}" name="Finish" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{FC6EB61C-7100-B448-9804-603C7E3ABEF3}" name="Start" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{E5228417-109C-A846-AF0B-030C79E6E401}" name="Finish" dataDxfId="27"/>
     <tableColumn id="6" xr3:uid="{0D84F3B2-D985-3649-8170-9FD8A89B6B7B}" name="Visual Flag"/>
     <tableColumn id="7" xr3:uid="{4DE64335-5CA3-C14F-836B-CE64DF9836EA}" name="Visual Swimlane"/>
     <tableColumn id="8" xr3:uid="{CF8C0B08-0C4D-E04F-9D8F-5EE6047AEC86}" name="Visual Track # Within Swimlane"/>
@@ -736,78 +751,81 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{95650287-5270-794F-BE83-228189F68705}" name="Table6" displayName="Table6" ref="O1:AM5" totalsRowShown="0">
-  <autoFilter ref="O1:AM5" xr:uid="{95650287-5270-794F-BE83-228189F68705}"/>
-  <tableColumns count="25">
-    <tableColumn id="1" xr3:uid="{A9D36371-651B-694F-A372-8CF380F533EC}" name="Num Visual Months" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{95650287-5270-794F-BE83-228189F68705}" name="Table6" displayName="Table6" ref="O1:AP5" totalsRowShown="0">
+  <autoFilter ref="O1:AP5" xr:uid="{95650287-5270-794F-BE83-228189F68705}"/>
+  <tableColumns count="28">
+    <tableColumn id="1" xr3:uid="{A9D36371-651B-694F-A372-8CF380F533EC}" name="Num Visual Months" dataDxfId="20">
       <calculatedColumnFormula>1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{52C6E4C9-BF49-3C41-BC4A-3E05A0279392}" name="Num Visual Days" dataDxfId="17">
+    <tableColumn id="9" xr3:uid="{52C6E4C9-BF49-3C41-BC4A-3E05A0279392}" name="Num Visual Days" dataDxfId="19">
       <calculatedColumnFormula>31</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{DC65A63A-00D1-A74D-A035-94831A6C664A}" name="Visual Start" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{DE63D43B-35E2-1D44-8D4E-E5E3760DF168}" name="Visual Finish" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{E8A718C3-23D8-CC4E-B23D-3EBE73F29401}" name="Visual Width" dataDxfId="22">
+    <tableColumn id="2" xr3:uid="{DC65A63A-00D1-A74D-A035-94831A6C664A}" name="Visual Start" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{DE63D43B-35E2-1D44-8D4E-E5E3760DF168}" name="Visual Finish" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{E8A718C3-23D8-CC4E-B23D-3EBE73F29401}" name="Visual Width" dataDxfId="24">
       <calculatedColumnFormula>Right-Left</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{CEF3950D-CB80-6044-B17D-B4B1A8490449}" name="Today" dataDxfId="13">
+    <tableColumn id="12" xr3:uid="{CEF3950D-CB80-6044-B17D-B4B1A8490449}" name="Today" dataDxfId="15">
       <calculatedColumnFormula>DATE(2021,1,5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{CB9DFFF7-900F-DF4E-A122-4CFDDA1F4267}" name="Day Width" dataDxfId="15">
+    <tableColumn id="5" xr3:uid="{CB9DFFF7-900F-DF4E-A122-4CFDDA1F4267}" name="Day Width" dataDxfId="17">
       <calculatedColumnFormula>Table6[[#This Row],[Visual Width]]/Table6[[#This Row],[Num Visual Days]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{4D076DCC-8A79-3943-9AD2-5D30AB20496A}" name="Points Per Cm" dataDxfId="12">
+    <tableColumn id="10" xr3:uid="{4D076DCC-8A79-3943-9AD2-5D30AB20496A}" name="Points Per Cm" dataDxfId="14">
       <calculatedColumnFormula>360000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{87B55787-4D49-F347-ACB4-0F290EE69403}" name="Num Shapes" dataDxfId="16">
+    <tableColumn id="17" xr3:uid="{87B55787-4D49-F347-ACB4-0F290EE69403}" name="Num Shapes" dataDxfId="18">
       <calculatedColumnFormula>IF(Table16[[#This Row],[Done Format String]]="",1,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{862BEB4E-A698-DC49-9CAA-B3C33191CD35}" name="Graphic 1 Days From Left" dataDxfId="21">
+    <tableColumn id="11" xr3:uid="{862BEB4E-A698-DC49-9CAA-B3C33191CD35}" name="Graphic 1 Days From Left" dataDxfId="23">
       <calculatedColumnFormula>Table16[[#This Row],[Start]]-Table6[[#This Row],[Visual Start]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{63C3F830-DD55-3F47-98B0-94365079404E}" name="Graphic 1 Top" dataDxfId="19">
+    <tableColumn id="6" xr3:uid="{63C3F830-DD55-3F47-98B0-94365079404E}" name="Graphic 1 Top" dataDxfId="21">
       <calculatedColumnFormula>ROUND((Top+(Table16[[#This Row],[Visual Track '# Within Swimlane]]-1)*(Track_Height+Track_Gap))*360000,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{2B754CAF-25BB-B64C-94DD-01B5925D7AC2}" name="Graphic 1 Left" dataDxfId="20">
+    <tableColumn id="7" xr3:uid="{2B754CAF-25BB-B64C-94DD-01B5925D7AC2}" name="Graphic 1 Left" dataDxfId="22">
       <calculatedColumnFormula>ROUND((Left+Table6[[#This Row],[Graphic 1 Days From Left]]*Table6[[#This Row],[Day Width]])*Table6[[#This Row],[Points Per Cm]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{3134E155-CCEA-6F4A-9ED4-2DEFCF056A3C}" name="Graphic 1 Width" dataDxfId="0">
+    <tableColumn id="25" xr3:uid="{3134E155-CCEA-6F4A-9ED4-2DEFCF056A3C}" name="Graphic 1 Width" dataDxfId="2">
       <calculatedColumnFormula>ROUND(IF(Table6[[#This Row],[Num Shapes]]=1,(Table16[[#This Row],[Finish]]-Table16[[#This Row],[Start]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]],(Table6[[#This Row],[Today]]-Table16[[#This Row],[Start]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]]),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{B236D0DC-FC55-3C4D-ABEE-6BEA9A987D2D}" name="Graphic 1 Export" dataDxfId="5">
+    <tableColumn id="28" xr3:uid="{911A5D55-8326-374F-8687-AB79F3FF6EF1}" name="Graphic 1 Height"/>
+    <tableColumn id="22" xr3:uid="{B236D0DC-FC55-3C4D-ABEE-6BEA9A987D2D}" name="Graphic 1 Export" dataDxfId="7">
       <calculatedColumnFormula>"("&amp;_xlfn.TEXTJOIN(", ",FALSE, Table6[[#This Row],[Graphic 1 Top]:[Graphic 1 Width]])&amp;")"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{7FD805D4-814F-2C44-9C12-67258071ABEE}" name="Graphic 2 Days From Left" dataDxfId="14">
+    <tableColumn id="13" xr3:uid="{7FD805D4-814F-2C44-9C12-67258071ABEE}" name="Graphic 2 Days From Left" dataDxfId="16">
       <calculatedColumnFormula>IF(Table6[[#This Row],[Num Shapes]]=1,"",Table6[[#This Row],[Today]]-Table6[[#This Row],[Visual Start]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{0ADBBF0F-A9D7-904E-A22E-A87D6B8B8D63}" name="Graphic 2 Top" dataDxfId="11">
+    <tableColumn id="15" xr3:uid="{0ADBBF0F-A9D7-904E-A22E-A87D6B8B8D63}" name="Graphic 2 Top" dataDxfId="13">
       <calculatedColumnFormula>IF(Table6[[#This Row],[Num Shapes]]=1,"",Table6[[#This Row],[Graphic 1 Top]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{CFED86F2-256C-E040-9909-052072892A44}" name="Graphic 2 Left" dataDxfId="10">
+    <tableColumn id="16" xr3:uid="{CFED86F2-256C-E040-9909-052072892A44}" name="Graphic 2 Left" dataDxfId="12">
       <calculatedColumnFormula>IF(Table6[[#This Row],[Num Shapes]]=1,"",ROUND((Left+Table6[[#This Row],[Graphic 2 Days From Left]]*Table6[[#This Row],[Day Width]])*Table6[[#This Row],[Points Per Cm]],0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{11DD9EDA-17D6-C74C-87A5-05BE6C12E5F2}" name="Graphic 2 Width" dataDxfId="1">
+    <tableColumn id="26" xr3:uid="{11DD9EDA-17D6-C74C-87A5-05BE6C12E5F2}" name="Graphic 2 Width" dataDxfId="3">
       <calculatedColumnFormula>IF(Table6[[#This Row],[Num Shapes]]=1,"",ROUND((Table16[[#This Row],[Finish]]-Table6[[#This Row],[Today]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]],0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{CD08D3CF-34D9-C84F-87E7-D4BBD2711218}" name="Graphic 2 Export" dataDxfId="4">
+    <tableColumn id="29" xr3:uid="{52361BE5-D180-684F-8869-3B29E31A32BC}" name="Graphic 2 Height" dataDxfId="1"/>
+    <tableColumn id="23" xr3:uid="{CD08D3CF-34D9-C84F-87E7-D4BBD2711218}" name="Graphic 2 Export" dataDxfId="6">
       <calculatedColumnFormula>IF(Table6[[#This Row],[Num Shapes]]=1,"","("&amp;_xlfn.TEXTJOIN(", ",FALSE, Table6[[#This Row],[Graphic 2 Top]:[Graphic 2 Width]])&amp;")")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{DD10CF7E-CB5E-F34B-AB3C-2FEF6D63CFC4}" name="Text Days From Left" dataDxfId="9">
+    <tableColumn id="18" xr3:uid="{DD10CF7E-CB5E-F34B-AB3C-2FEF6D63CFC4}" name="Text Days From Left" dataDxfId="11">
       <calculatedColumnFormula>Table16[[#This Row],[Start]]-Table6[[#This Row],[Visual Start]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{251D2619-6DAD-1045-B9A0-8BDEE9B82806}" name="Text Top" dataDxfId="8">
+    <tableColumn id="19" xr3:uid="{251D2619-6DAD-1045-B9A0-8BDEE9B82806}" name="Text Top" dataDxfId="10">
       <calculatedColumnFormula>ROUND((Top+(Table16[[#This Row],[Visual Track '# Within Swimlane]]-1)*(Track_Height+Track_Gap))*360000,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{013082E2-ECB6-D649-A1F4-0CDEE6D50347}" name="Text Left" dataDxfId="7">
+    <tableColumn id="20" xr3:uid="{013082E2-ECB6-D649-A1F4-0CDEE6D50347}" name="Text Left" dataDxfId="9">
       <calculatedColumnFormula>ROUND((Left+Table6[[#This Row],[Graphic 1 Days From Left]]*Table6[[#This Row],[Day Width]])*Table6[[#This Row],[Points Per Cm]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{CC791E80-A6A4-1C4F-8038-8C67770BD828}" name="Text Width" dataDxfId="2">
+    <tableColumn id="27" xr3:uid="{CC791E80-A6A4-1C4F-8038-8C67770BD828}" name="Text Width" dataDxfId="4">
       <calculatedColumnFormula>ROUND((Table16[[#This Row],[Finish]]-Table16[[#This Row],[Start]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{BC99535B-484E-854F-AA07-93A4E18F8797}" name="Text Export" dataDxfId="3">
+    <tableColumn id="30" xr3:uid="{D437B0B7-7561-224C-B00A-43251989860C}" name="Text Height" dataDxfId="0"/>
+    <tableColumn id="24" xr3:uid="{BC99535B-484E-854F-AA07-93A4E18F8797}" name="Text Export" dataDxfId="5">
       <calculatedColumnFormula>"("&amp;_xlfn.TEXTJOIN(", ",FALSE, Table6[[#This Row],[Text Top]:[Text Width]])&amp;")"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{62743F9D-847D-3F4E-BC1E-B073C3B3E68A}" name="Export To Python Test Suite" dataDxfId="6">
+    <tableColumn id="21" xr3:uid="{62743F9D-847D-3F4E-BC1E-B073C3B3E68A}" name="Graphic 1 Top, Graphic 1 Left, Graphic 1 Width, Graphic 2 Top, Graphic 2 Left, Graphic 2 Width, Text Top, Text Left, Text Width" dataDxfId="8">
       <calculatedColumnFormula>"("&amp;"""Activity"""&amp;", "&amp;""""&amp;Table16[[#This Row],[Task Name]]&amp;""""&amp;", "&amp;"["&amp;_xlfn.TEXTJOIN(", ",TRUE, Table6[[#This Row],[Graphic 1 Export]],Table6[[#This Row],[Graphic 2 Export]],Table6[[#This Row],[Text Export]])&amp;"]"&amp;"),"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1234,7 +1252,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView zoomScale="172" workbookViewId="0">
+    <sheetView topLeftCell="I1" zoomScale="172" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -2104,9 +2122,9 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AM5"/>
+  <dimension ref="A1:AP5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="182" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="182" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -2136,23 +2154,23 @@
     <col min="24" max="24" width="25" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="15" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.1640625" customWidth="1"/>
-    <col min="28" max="28" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="25" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="15.1640625" customWidth="1"/>
-    <col min="33" max="33" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11" customWidth="1"/>
-    <col min="38" max="38" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="97.83203125" bestFit="1" customWidth="1"/>
-    <col min="40" max="106" width="3.33203125" customWidth="1"/>
+    <col min="27" max="28" width="15.1640625" customWidth="1"/>
+    <col min="29" max="29" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="25" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="34" width="15.1640625" customWidth="1"/>
+    <col min="35" max="35" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11" bestFit="1" customWidth="1"/>
+    <col min="39" max="40" width="11" customWidth="1"/>
+    <col min="41" max="41" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="110.6640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="109" width="3.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>78</v>
       </c>
@@ -2217,55 +2235,64 @@
         <v>88</v>
       </c>
       <c r="X1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z1" t="s">
         <v>91</v>
       </c>
-      <c r="Y1" t="s">
-        <v>90</v>
-      </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AC1" t="s">
         <v>92</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AD1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AG1" t="s">
         <v>102</v>
       </c>
-      <c r="AB1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AE1" t="s">
+      <c r="AH1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI1" t="s">
         <v>96</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AJ1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AM1" t="s">
         <v>103</v>
       </c>
-      <c r="AG1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AJ1" t="s">
+      <c r="AN1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AO1" t="s">
         <v>99</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AP1" t="s">
         <v>104</v>
       </c>
-      <c r="AL1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -2282,6 +2309,9 @@
         <v>62</v>
       </c>
       <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
         <v>1</v>
       </c>
       <c r="J2" t="s">
@@ -2340,56 +2370,58 @@
         <f>ROUND(IF(Table6[[#This Row],[Num Shapes]]=1,(Table16[[#This Row],[Finish]]-Table16[[#This Row],[Start]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]],(Table6[[#This Row],[Today]]-Table16[[#This Row],[Start]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]]),0)</f>
         <v>11103097</v>
       </c>
-      <c r="AB2" t="str">
+      <c r="AC2" t="str">
         <f>"("&amp;_xlfn.TEXTJOIN(", ",FALSE, Table6[[#This Row],[Graphic 1 Top]:[Graphic 1 Width]])&amp;")"</f>
         <v>(360000, 720000, 11103097)</v>
       </c>
-      <c r="AC2" s="7" t="str">
+      <c r="AD2" s="7" t="str">
         <f>IF(Table6[[#This Row],[Num Shapes]]=1,"",Table6[[#This Row],[Today]]-Table6[[#This Row],[Visual Start]])</f>
         <v/>
       </c>
-      <c r="AD2" s="7" t="str">
+      <c r="AE2" s="7" t="str">
         <f>IF(Table6[[#This Row],[Num Shapes]]=1,"",Table6[[#This Row],[Graphic 1 Top]])</f>
         <v/>
       </c>
-      <c r="AE2" s="7" t="str">
+      <c r="AF2" s="7" t="str">
         <f>IF(Table6[[#This Row],[Num Shapes]]=1,"",ROUND((Left+Table6[[#This Row],[Graphic 2 Days From Left]]*Table6[[#This Row],[Day Width]])*Table6[[#This Row],[Points Per Cm]],0))</f>
         <v/>
       </c>
-      <c r="AF2" s="7" t="str">
+      <c r="AG2" s="7" t="str">
         <f>IF(Table6[[#This Row],[Num Shapes]]=1,"",ROUND((Table16[[#This Row],[Finish]]-Table6[[#This Row],[Today]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]],0))</f>
         <v/>
       </c>
-      <c r="AG2" t="str">
+      <c r="AH2" s="7"/>
+      <c r="AI2" t="str">
         <f>IF(Table6[[#This Row],[Num Shapes]]=1,"","("&amp;_xlfn.TEXTJOIN(", ",FALSE, Table6[[#This Row],[Graphic 2 Top]:[Graphic 2 Width]])&amp;")")</f>
         <v/>
       </c>
-      <c r="AH2" s="7">
+      <c r="AJ2" s="7">
         <f>Table16[[#This Row],[Start]]-Table6[[#This Row],[Visual Start]]</f>
         <v>0</v>
       </c>
-      <c r="AI2" s="7">
+      <c r="AK2" s="7">
         <f>ROUND((Top+(Table16[[#This Row],[Visual Track '# Within Swimlane]]-1)*(Track_Height+Track_Gap))*360000,0)</f>
         <v>360000</v>
       </c>
-      <c r="AJ2" s="7">
+      <c r="AL2" s="7">
         <f>ROUND((Left+Table6[[#This Row],[Graphic 1 Days From Left]]*Table6[[#This Row],[Day Width]])*Table6[[#This Row],[Points Per Cm]],0)</f>
         <v>720000</v>
       </c>
-      <c r="AK2" s="7">
+      <c r="AM2" s="7">
         <f>ROUND((Table16[[#This Row],[Finish]]-Table16[[#This Row],[Start]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]],0)</f>
         <v>11103097</v>
       </c>
-      <c r="AL2" s="7" t="str">
+      <c r="AN2" s="7"/>
+      <c r="AO2" s="7" t="str">
         <f>"("&amp;_xlfn.TEXTJOIN(", ",FALSE, Table6[[#This Row],[Text Top]:[Text Width]])&amp;")"</f>
         <v>(360000, 720000, 11103097)</v>
       </c>
-      <c r="AM2" s="7" t="str">
+      <c r="AP2" s="7" t="str">
         <f>"("&amp;"""Activity"""&amp;", "&amp;""""&amp;Table16[[#This Row],[Task Name]]&amp;""""&amp;", "&amp;"["&amp;_xlfn.TEXTJOIN(", ",TRUE, Table6[[#This Row],[Graphic 1 Export]],Table6[[#This Row],[Graphic 2 Export]],Table6[[#This Row],[Text Export]])&amp;"]"&amp;"),"</f>
         <v>("Activity", "Activity 01", [(360000, 720000, 11103097), (360000, 720000, 11103097)]),</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>65</v>
       </c>
@@ -2406,6 +2438,9 @@
         <v>62</v>
       </c>
       <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
         <v>2</v>
       </c>
       <c r="J3" t="s">
@@ -2464,56 +2499,58 @@
         <f>ROUND(IF(Table6[[#This Row],[Num Shapes]]=1,(Table16[[#This Row],[Finish]]-Table16[[#This Row],[Start]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]],(Table6[[#This Row],[Today]]-Table16[[#This Row],[Start]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]]),0)</f>
         <v>11103097</v>
       </c>
-      <c r="AB3" t="str">
+      <c r="AC3" t="str">
         <f>"("&amp;_xlfn.TEXTJOIN(", ",FALSE, Table6[[#This Row],[Graphic 1 Top]:[Graphic 1 Width]])&amp;")"</f>
         <v>(576000, 720000, 11103097)</v>
       </c>
-      <c r="AC3" s="7" t="str">
+      <c r="AD3" s="7" t="str">
         <f>IF(Table6[[#This Row],[Num Shapes]]=1,"",Table6[[#This Row],[Today]]-Table6[[#This Row],[Visual Start]])</f>
         <v/>
       </c>
-      <c r="AD3" s="7" t="str">
+      <c r="AE3" s="7" t="str">
         <f>IF(Table6[[#This Row],[Num Shapes]]=1,"",Table6[[#This Row],[Graphic 1 Top]])</f>
         <v/>
       </c>
-      <c r="AE3" s="7" t="str">
+      <c r="AF3" s="7" t="str">
         <f>IF(Table6[[#This Row],[Num Shapes]]=1,"",ROUND((Left+Table6[[#This Row],[Graphic 2 Days From Left]]*Table6[[#This Row],[Day Width]])*Table6[[#This Row],[Points Per Cm]],0))</f>
         <v/>
       </c>
-      <c r="AF3" s="7" t="str">
+      <c r="AG3" s="7" t="str">
         <f>IF(Table6[[#This Row],[Num Shapes]]=1,"",ROUND((Table16[[#This Row],[Finish]]-Table6[[#This Row],[Today]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]],0))</f>
         <v/>
       </c>
-      <c r="AG3" s="7" t="str">
+      <c r="AH3" s="7"/>
+      <c r="AI3" s="7" t="str">
         <f>IF(Table6[[#This Row],[Num Shapes]]=1,"","("&amp;_xlfn.TEXTJOIN(", ",FALSE, Table6[[#This Row],[Graphic 2 Top]:[Graphic 2 Width]])&amp;")")</f>
         <v/>
       </c>
-      <c r="AH3" s="7">
+      <c r="AJ3" s="7">
         <f>Table16[[#This Row],[Start]]-Table6[[#This Row],[Visual Start]]</f>
         <v>0</v>
       </c>
-      <c r="AI3" s="7">
+      <c r="AK3" s="7">
         <f>ROUND((Top+(Table16[[#This Row],[Visual Track '# Within Swimlane]]-1)*(Track_Height+Track_Gap))*360000,0)</f>
         <v>576000</v>
       </c>
-      <c r="AJ3" s="7">
+      <c r="AL3" s="7">
         <f>ROUND((Left+Table6[[#This Row],[Graphic 1 Days From Left]]*Table6[[#This Row],[Day Width]])*Table6[[#This Row],[Points Per Cm]],0)</f>
         <v>720000</v>
       </c>
-      <c r="AK3" s="7">
+      <c r="AM3" s="7">
         <f>ROUND((Table16[[#This Row],[Finish]]-Table16[[#This Row],[Start]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]],0)</f>
         <v>11103097</v>
       </c>
-      <c r="AL3" s="7" t="str">
+      <c r="AN3" s="7"/>
+      <c r="AO3" s="7" t="str">
         <f>"("&amp;_xlfn.TEXTJOIN(", ",FALSE, Table6[[#This Row],[Text Top]:[Text Width]])&amp;")"</f>
         <v>(576000, 720000, 11103097)</v>
       </c>
-      <c r="AM3" s="7" t="str">
+      <c r="AP3" s="7" t="str">
         <f>"("&amp;"""Activity"""&amp;", "&amp;""""&amp;Table16[[#This Row],[Task Name]]&amp;""""&amp;", "&amp;"["&amp;_xlfn.TEXTJOIN(", ",TRUE, Table6[[#This Row],[Graphic 1 Export]],Table6[[#This Row],[Graphic 2 Export]],Table6[[#This Row],[Text Export]])&amp;"]"&amp;"),"</f>
         <v>("Activity", "Activity 02", [(576000, 720000, 11103097), (576000, 720000, 11103097)]),</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -2530,6 +2567,9 @@
         <v>62</v>
       </c>
       <c r="H4">
+        <v>4</v>
+      </c>
+      <c r="I4">
         <v>3</v>
       </c>
       <c r="J4" t="s">
@@ -2578,7 +2618,7 @@
       </c>
       <c r="Y4">
         <f>ROUND((Top+(Table16[[#This Row],[Visual Track '# Within Swimlane]]-1)*(Track_Height+Track_Gap))*360000,0)</f>
-        <v>792000</v>
+        <v>1008000</v>
       </c>
       <c r="Z4">
         <f>ROUND((Left+Table6[[#This Row],[Graphic 1 Days From Left]]*Table6[[#This Row],[Day Width]])*Table6[[#This Row],[Points Per Cm]],0)</f>
@@ -2588,56 +2628,58 @@
         <f>ROUND(IF(Table6[[#This Row],[Num Shapes]]=1,(Table16[[#This Row],[Finish]]-Table16[[#This Row],[Start]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]],(Table6[[#This Row],[Today]]-Table16[[#This Row],[Start]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]]),0)</f>
         <v>10732994</v>
       </c>
-      <c r="AB4" t="str">
+      <c r="AC4" t="str">
         <f>"("&amp;_xlfn.TEXTJOIN(", ",FALSE, Table6[[#This Row],[Graphic 1 Top]:[Graphic 1 Width]])&amp;")"</f>
-        <v>(792000, 1090103, 10732994)</v>
-      </c>
-      <c r="AC4" s="7" t="str">
+        <v>(1008000, 1090103, 10732994)</v>
+      </c>
+      <c r="AD4" s="7" t="str">
         <f>IF(Table6[[#This Row],[Num Shapes]]=1,"",Table6[[#This Row],[Today]]-Table6[[#This Row],[Visual Start]])</f>
         <v/>
       </c>
-      <c r="AD4" s="7" t="str">
+      <c r="AE4" s="7" t="str">
         <f>IF(Table6[[#This Row],[Num Shapes]]=1,"",Table6[[#This Row],[Graphic 1 Top]])</f>
         <v/>
       </c>
-      <c r="AE4" s="7" t="str">
+      <c r="AF4" s="7" t="str">
         <f>IF(Table6[[#This Row],[Num Shapes]]=1,"",ROUND((Left+Table6[[#This Row],[Graphic 2 Days From Left]]*Table6[[#This Row],[Day Width]])*Table6[[#This Row],[Points Per Cm]],0))</f>
         <v/>
       </c>
-      <c r="AF4" s="7" t="str">
+      <c r="AG4" s="7" t="str">
         <f>IF(Table6[[#This Row],[Num Shapes]]=1,"",ROUND((Table16[[#This Row],[Finish]]-Table6[[#This Row],[Today]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]],0))</f>
         <v/>
       </c>
-      <c r="AG4" s="7" t="str">
+      <c r="AH4" s="7"/>
+      <c r="AI4" s="7" t="str">
         <f>IF(Table6[[#This Row],[Num Shapes]]=1,"","("&amp;_xlfn.TEXTJOIN(", ",FALSE, Table6[[#This Row],[Graphic 2 Top]:[Graphic 2 Width]])&amp;")")</f>
         <v/>
       </c>
-      <c r="AH4" s="7">
+      <c r="AJ4" s="7">
         <f>Table16[[#This Row],[Start]]-Table6[[#This Row],[Visual Start]]</f>
         <v>1</v>
       </c>
-      <c r="AI4" s="7">
+      <c r="AK4" s="7">
         <f>ROUND((Top+(Table16[[#This Row],[Visual Track '# Within Swimlane]]-1)*(Track_Height+Track_Gap))*360000,0)</f>
-        <v>792000</v>
-      </c>
-      <c r="AJ4" s="7">
+        <v>1008000</v>
+      </c>
+      <c r="AL4" s="7">
         <f>ROUND((Left+Table6[[#This Row],[Graphic 1 Days From Left]]*Table6[[#This Row],[Day Width]])*Table6[[#This Row],[Points Per Cm]],0)</f>
         <v>1090103</v>
       </c>
-      <c r="AK4" s="7">
+      <c r="AM4" s="7">
         <f>ROUND((Table16[[#This Row],[Finish]]-Table16[[#This Row],[Start]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]],0)</f>
         <v>10732994</v>
       </c>
-      <c r="AL4" s="7" t="str">
+      <c r="AN4" s="7"/>
+      <c r="AO4" s="7" t="str">
         <f>"("&amp;_xlfn.TEXTJOIN(", ",FALSE, Table6[[#This Row],[Text Top]:[Text Width]])&amp;")"</f>
-        <v>(792000, 1090103, 10732994)</v>
-      </c>
-      <c r="AM4" s="7" t="str">
+        <v>(1008000, 1090103, 10732994)</v>
+      </c>
+      <c r="AP4" s="7" t="str">
         <f>"("&amp;"""Activity"""&amp;", "&amp;""""&amp;Table16[[#This Row],[Task Name]]&amp;""""&amp;", "&amp;"["&amp;_xlfn.TEXTJOIN(", ",TRUE, Table6[[#This Row],[Graphic 1 Export]],Table6[[#This Row],[Graphic 2 Export]],Table6[[#This Row],[Text Export]])&amp;"]"&amp;"),"</f>
-        <v>("Activity", "Activity 03", [(792000, 1090103, 10732994), (792000, 1090103, 10732994)]),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.2">
+        <v>("Activity", "Activity 03", [(1008000, 1090103, 10732994), (1008000, 1090103, 10732994)]),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -2654,7 +2696,10 @@
         <v>62</v>
       </c>
       <c r="H5">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
       </c>
       <c r="J5" t="s">
         <v>63</v>
@@ -2705,7 +2750,7 @@
       </c>
       <c r="Y5" s="7">
         <f>ROUND((Top+(Table16[[#This Row],[Visual Track '# Within Swimlane]]-1)*(Track_Height+Track_Gap))*360000,0)</f>
-        <v>1008000</v>
+        <v>1656000</v>
       </c>
       <c r="Z5" s="7">
         <f>ROUND((Left+Table6[[#This Row],[Graphic 1 Days From Left]]*Table6[[#This Row],[Day Width]])*Table6[[#This Row],[Points Per Cm]],0)</f>
@@ -2715,53 +2760,56 @@
         <f>ROUND(IF(Table6[[#This Row],[Num Shapes]]=1,(Table16[[#This Row],[Finish]]-Table16[[#This Row],[Start]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]],(Table6[[#This Row],[Today]]-Table16[[#This Row],[Start]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]]),0)</f>
         <v>1110310</v>
       </c>
-      <c r="AB5" s="7" t="str">
+      <c r="AB5" s="7"/>
+      <c r="AC5" s="7" t="str">
         <f>"("&amp;_xlfn.TEXTJOIN(", ",FALSE, Table6[[#This Row],[Graphic 1 Top]:[Graphic 1 Width]])&amp;")"</f>
-        <v>(1008000, 1460206, 1110310)</v>
-      </c>
-      <c r="AC5" s="7">
+        <v>(1656000, 1460206, 1110310)</v>
+      </c>
+      <c r="AD5" s="7">
         <f>IF(Table6[[#This Row],[Num Shapes]]=1,"",Table6[[#This Row],[Today]]-Table6[[#This Row],[Visual Start]])</f>
         <v>4</v>
       </c>
-      <c r="AD5" s="7">
+      <c r="AE5" s="7">
         <f>IF(Table6[[#This Row],[Num Shapes]]=1,"",Table6[[#This Row],[Graphic 1 Top]])</f>
-        <v>1008000</v>
-      </c>
-      <c r="AE5" s="7">
+        <v>1656000</v>
+      </c>
+      <c r="AF5" s="7">
         <f>IF(Table6[[#This Row],[Num Shapes]]=1,"",ROUND((Left+Table6[[#This Row],[Graphic 2 Days From Left]]*Table6[[#This Row],[Day Width]])*Table6[[#This Row],[Points Per Cm]],0))</f>
         <v>2200413</v>
       </c>
-      <c r="AF5" s="7">
+      <c r="AG5" s="7">
         <f>IF(Table6[[#This Row],[Num Shapes]]=1,"",ROUND((Table16[[#This Row],[Finish]]-Table6[[#This Row],[Today]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]],0))</f>
         <v>5921652</v>
       </c>
-      <c r="AG5" s="7" t="str">
+      <c r="AH5" s="7"/>
+      <c r="AI5" s="7" t="str">
         <f>IF(Table6[[#This Row],[Num Shapes]]=1,"","("&amp;_xlfn.TEXTJOIN(", ",FALSE, Table6[[#This Row],[Graphic 2 Top]:[Graphic 2 Width]])&amp;")")</f>
-        <v>(1008000, 2200413, 5921652)</v>
-      </c>
-      <c r="AH5" s="7">
+        <v>(1656000, 2200413, 5921652)</v>
+      </c>
+      <c r="AJ5" s="7">
         <f>Table16[[#This Row],[Start]]-Table6[[#This Row],[Visual Start]]</f>
         <v>2</v>
       </c>
-      <c r="AI5" s="7">
+      <c r="AK5" s="7">
         <f>ROUND((Top+(Table16[[#This Row],[Visual Track '# Within Swimlane]]-1)*(Track_Height+Track_Gap))*360000,0)</f>
-        <v>1008000</v>
-      </c>
-      <c r="AJ5" s="7">
+        <v>1656000</v>
+      </c>
+      <c r="AL5" s="7">
         <f>ROUND((Left+Table6[[#This Row],[Graphic 1 Days From Left]]*Table6[[#This Row],[Day Width]])*Table6[[#This Row],[Points Per Cm]],0)</f>
         <v>1460206</v>
       </c>
-      <c r="AK5" s="7">
+      <c r="AM5" s="7">
         <f>ROUND((Table16[[#This Row],[Finish]]-Table16[[#This Row],[Start]]+1)*Table6[[#This Row],[Day Width]]*Table6[[#This Row],[Points Per Cm]],0)</f>
         <v>6661858</v>
       </c>
-      <c r="AL5" s="7" t="str">
+      <c r="AN5" s="7"/>
+      <c r="AO5" s="7" t="str">
         <f>"("&amp;_xlfn.TEXTJOIN(", ",FALSE, Table6[[#This Row],[Text Top]:[Text Width]])&amp;")"</f>
-        <v>(1008000, 1460206, 6661858)</v>
-      </c>
-      <c r="AM5" s="7" t="str">
+        <v>(1656000, 1460206, 6661858)</v>
+      </c>
+      <c r="AP5" s="7" t="str">
         <f>"("&amp;"""Activity"""&amp;", "&amp;""""&amp;Table16[[#This Row],[Task Name]]&amp;""""&amp;", "&amp;"["&amp;_xlfn.TEXTJOIN(", ",TRUE, Table6[[#This Row],[Graphic 1 Export]],Table6[[#This Row],[Graphic 2 Export]],Table6[[#This Row],[Text Export]])&amp;"]"&amp;"),"</f>
-        <v>("Activity", "Activity 04", [(1008000, 1460206, 1110310), (1008000, 2200413, 5921652), (1008000, 1460206, 6661858)]),</v>
+        <v>("Activity", "Activity 04", [(1656000, 1460206, 1110310), (1656000, 2200413, 5921652), (1656000, 1460206, 6661858)]),</v>
       </c>
     </row>
   </sheetData>

</xml_diff>